<commit_message>
Planilha de testes atualizada
</commit_message>
<xml_diff>
--- a/documents/Sprint-03/planilhaTeste/Plano de UAT - HML v1.xlsx
+++ b/documents/Sprint-03/planilhaTeste/Plano de UAT - HML v1.xlsx
@@ -1,35 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Projeto-3Semetre\simplify\documents\Sprint-03\planilhaTeste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCBD7A5-3906-4EFD-8F75-EC35BA6771D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="503"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cenário - Pesquisar Cliente" sheetId="6" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
   <si>
     <t xml:space="preserve">Projeto: </t>
   </si>
@@ -412,15 +403,42 @@
   <si>
     <t>Ao clicar o cliente deve efetuar o login na nossa aplicação</t>
   </si>
+  <si>
+    <t xml:space="preserve">Não ok. </t>
+  </si>
+  <si>
+    <t>Ok.</t>
+  </si>
+  <si>
+    <t>Não ok.</t>
+  </si>
+  <si>
+    <t>Não ok. Ao selecionar um serviço ele não é redirecionado</t>
+  </si>
+  <si>
+    <t>Não ok. Não gera nenhum arquivo ou resultado</t>
+  </si>
+  <si>
+    <t>Não ok. Sem máscara para email.</t>
+  </si>
+  <si>
+    <t>Não ok</t>
+  </si>
+  <si>
+    <t>Não ok. Não aparece checkbox.</t>
+  </si>
+  <si>
+    <t>Ok com 1 defeito</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -466,13 +484,6 @@
       <b/>
       <sz val="12"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -706,13 +717,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="12" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -743,7 +750,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -751,32 +758,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -793,11 +789,11 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -809,26 +805,26 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -840,7 +836,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -848,43 +844,47 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Background" xfId="1"/>
-    <cellStyle name="Card" xfId="2"/>
-    <cellStyle name="Card B" xfId="3"/>
-    <cellStyle name="Card BL" xfId="4"/>
-    <cellStyle name="Card BR" xfId="5"/>
-    <cellStyle name="Card L" xfId="6"/>
-    <cellStyle name="Card R" xfId="7"/>
-    <cellStyle name="Card T" xfId="8"/>
-    <cellStyle name="Card TL" xfId="9"/>
-    <cellStyle name="Card TR" xfId="10"/>
-    <cellStyle name="Column Header" xfId="11"/>
+    <cellStyle name="Background" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Card" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Card B" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Card BL" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Card BR" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Card L" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Card R" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Card T" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Card TL" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Card TR" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Column Header" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Hiperlink" xfId="12" builtinId="8"/>
-    <cellStyle name="Input" xfId="13"/>
+    <cellStyle name="Input" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="14"/>
+    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1043,6 +1043,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1078,6 +1095,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1253,907 +1287,1086 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="4" customWidth="1"/>
-    <col min="9" max="10" width="20.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="32.28515625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" style="4" customWidth="1"/>
-    <col min="18" max="16384" width="11.7109375" style="4"/>
+    <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="20.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="32.28515625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="11.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>44146</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
+    <row r="17" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B17" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="K17" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-    </row>
-    <row r="18" spans="2:21" s="13" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="12">
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+    </row>
+    <row r="18" spans="2:21" s="12" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="11">
         <v>1</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="18"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-    </row>
-    <row r="19" spans="2:21" s="13" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="12">
+      <c r="I18" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+    </row>
+    <row r="19" spans="2:21" s="12" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="11">
         <v>2</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-    </row>
-    <row r="20" spans="2:21" s="13" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="12">
+      <c r="J19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+    </row>
+    <row r="20" spans="2:21" s="12" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11">
         <v>3</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-    </row>
-    <row r="21" spans="2:21" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="B21" s="12">
+      <c r="J20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+    </row>
+    <row r="21" spans="2:21" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+      <c r="B21" s="11">
         <v>4</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-    </row>
-    <row r="22" spans="2:21" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B22" s="12">
+      <c r="J21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+    </row>
+    <row r="22" spans="2:21" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="B22" s="11">
         <v>5</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-    </row>
-    <row r="23" spans="2:21" s="13" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="12">
+      <c r="J22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+    </row>
+    <row r="23" spans="2:21" s="12" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="11">
         <v>6</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="1"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-    </row>
-    <row r="24" spans="2:21" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B24" s="12">
+      <c r="I23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+    </row>
+    <row r="24" spans="2:21" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B24" s="11">
         <v>7</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="1"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-    </row>
-    <row r="25" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B25" s="12">
+      <c r="H24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+    </row>
+    <row r="25" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B25" s="11">
         <v>8</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="1"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-    </row>
-    <row r="26" spans="2:21" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="B26" s="28" t="s">
+      <c r="G25" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I25" s="15"/>
+      <c r="J25" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+    </row>
+    <row r="26" spans="2:21" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B26" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="1"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-    </row>
-    <row r="27" spans="2:21" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B27" s="28" t="s">
+      <c r="G26" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+    </row>
+    <row r="27" spans="2:21" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B27" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="1"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-    </row>
-    <row r="28" spans="2:21" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="B28" s="12">
+      <c r="G27" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+    </row>
+    <row r="28" spans="2:21" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="B28" s="11">
         <v>9</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="16"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="1"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-    </row>
-    <row r="29" spans="2:21" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B29" s="28" t="s">
+      <c r="G28" s="15"/>
+      <c r="H28" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+    </row>
+    <row r="29" spans="2:21" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B29" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-    </row>
-    <row r="30" spans="2:21" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="B30" s="28" t="s">
+      <c r="G29" s="15"/>
+      <c r="H29" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+    </row>
+    <row r="30" spans="2:21" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="B30" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="1"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="14"/>
-    </row>
-    <row r="31" spans="2:21" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B31" s="28" t="s">
+      <c r="G30" s="15"/>
+      <c r="H30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+    </row>
+    <row r="31" spans="2:21" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B31" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="1"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="14"/>
-    </row>
-    <row r="32" spans="2:21" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B32" s="28" t="s">
+      <c r="G31" s="15"/>
+      <c r="H31" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+    </row>
+    <row r="32" spans="2:21" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B32" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="1"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="14"/>
-    </row>
-    <row r="33" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B33" s="29">
+      <c r="G32" s="15"/>
+      <c r="H32" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+    </row>
+    <row r="33" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B33" s="25">
         <v>10</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="1"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="14"/>
-    </row>
-    <row r="34" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B34" s="41" t="s">
+      <c r="G33" s="15"/>
+      <c r="H33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+    </row>
+    <row r="34" spans="2:21" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B34" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F34" s="42" t="s">
+      <c r="F34" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="1"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="14"/>
-    </row>
-    <row r="35" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B35" s="41" t="s">
+      <c r="G34" s="15"/>
+      <c r="H34" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+    </row>
+    <row r="35" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B35" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="42" t="s">
+      <c r="F35" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="G35" s="16"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="1"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
-      <c r="U35" s="14"/>
-    </row>
-    <row r="36" spans="2:21" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="B36" s="41">
+      <c r="G35" s="15"/>
+      <c r="H35" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+    </row>
+    <row r="36" spans="2:21" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="B36" s="36">
         <v>11</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="42" t="s">
+      <c r="D36" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="42" t="s">
+      <c r="F36" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="G36" s="16"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="1"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
-      <c r="T36" s="14"/>
-      <c r="U36" s="14"/>
-    </row>
-    <row r="37" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B37" s="41" t="s">
+      <c r="G36" s="15"/>
+      <c r="H36" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+    </row>
+    <row r="37" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B37" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="42" t="s">
+      <c r="F37" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="16"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="1"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-    </row>
-    <row r="38" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B38" s="41" t="s">
+      <c r="G37" s="15"/>
+      <c r="H37" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+    </row>
+    <row r="38" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B38" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42" t="s">
+      <c r="E38" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="G38" s="16"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="1"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-    </row>
-    <row r="39" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B39" s="41">
+      <c r="G38" s="15"/>
+      <c r="H38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+    </row>
+    <row r="39" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B39" s="36">
         <v>12</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="42" t="s">
+      <c r="F39" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="G39" s="16"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="1"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
-      <c r="T39" s="14"/>
-      <c r="U39" s="14"/>
-    </row>
-    <row r="40" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B40" s="41" t="s">
+      <c r="G39" s="15"/>
+      <c r="H39" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+    </row>
+    <row r="40" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B40" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="42" t="s">
+      <c r="D40" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42" t="s">
+      <c r="E40" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G40" s="16"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="1"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-    </row>
-    <row r="41" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B41" s="41" t="s">
+      <c r="G40" s="15"/>
+      <c r="H40" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+    </row>
+    <row r="41" spans="2:21" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B41" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42" t="s">
+      <c r="E41" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="1"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="14"/>
-    </row>
-    <row r="42" spans="2:21" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="B42" s="12" t="s">
+      <c r="G41" s="15"/>
+      <c r="H41" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I41" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+    </row>
+    <row r="42" spans="2:21" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B42" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="1"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-    </row>
-    <row r="43" spans="2:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="34"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-    </row>
-    <row r="44" spans="2:21" s="13" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
-      <c r="U44" s="14"/>
-    </row>
-    <row r="45" spans="2:21" s="13" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="14"/>
-      <c r="U45" s="14"/>
-    </row>
-    <row r="46" spans="2:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="E46" s="39"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
-      <c r="T46" s="14"/>
-      <c r="U46" s="14"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+    </row>
+    <row r="43" spans="2:21" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="30"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+    </row>
+    <row r="44" spans="2:21" s="12" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+    </row>
+    <row r="45" spans="2:21" s="12" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+    </row>
+    <row r="46" spans="2:21" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="E46" s="35"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="18">
         <v>43903</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B53" s="9"/>
+      <c r="B53" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C8:D8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G18" r:id="rId1"/>
-    <hyperlink ref="G19" r:id="rId2"/>
-    <hyperlink ref="G20" r:id="rId3"/>
-    <hyperlink ref="G21" r:id="rId4"/>
-    <hyperlink ref="G22" r:id="rId5"/>
-    <hyperlink ref="G23" r:id="rId6"/>
-    <hyperlink ref="G24" r:id="rId7"/>
+    <hyperlink ref="G18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G21" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G22" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G23" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G24" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G25:G30" r:id="rId8" display="https://www.figma.com/file/D9IcJBTqi47t62lUJY9C4r/Simplify?node-id=27%3A3" xr:uid="{D5F60EF0-09D2-48F4-92A5-7901B7C84F9F}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
-  <pageSetup fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>

</xml_diff>